<commit_message>
Week  27/5/2018 To 6/3/2018
</commit_message>
<xml_diff>
--- a/Working Progress Timetable/Time sheet 1.xlsx
+++ b/Working Progress Timetable/Time sheet 1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Report Duration</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>Read TensorFlow: A system for large-scale machine learning</t>
+  </si>
+  <si>
+    <t>Hands on</t>
+  </si>
+  <si>
+    <t>Reading</t>
   </si>
 </sst>
 </file>
@@ -112,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,6 +155,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -272,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -302,6 +314,18 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -317,17 +341,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D11" sqref="D11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -650,11 +674,11 @@
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.6" customHeight="1" thickBot="1">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:11" ht="33.6" customHeight="1" thickBot="1">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="16"/>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
@@ -668,7 +692,7 @@
         <v>43137</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.4">
+    <row r="2" spans="1:11" ht="14.4">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -676,251 +700,259 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="33.6" customHeight="1">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14" t="s">
+    <row r="3" spans="1:11" ht="33.6" customHeight="1">
+      <c r="A3" s="17"/>
+      <c r="B3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="1:6" ht="24.6" customHeight="1">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:11" ht="24.6" customHeight="1">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="I4" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1">
       <c r="A5" s="7">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="9">
-        <v>10</v>
-      </c>
-      <c r="D5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
+      <c r="D5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1">
       <c r="A6" s="10">
         <v>2</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="10">
         <v>6</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1">
       <c r="A7" s="7">
         <v>3</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="9">
         <v>5</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1">
+      <c r="E7" s="13"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1">
       <c r="A8" s="10">
         <v>4</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="21" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="10">
         <v>3</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1">
+      <c r="E8" s="13"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1">
       <c r="A9" s="9">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="9">
         <v>7</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" ht="14.4">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" ht="14.4">
       <c r="A10" s="7">
         <v>7</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="9">
         <v>10</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="1:6" ht="14.4">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" ht="14.4">
       <c r="A11" s="10">
         <v>8</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="10">
-        <v>1</v>
-      </c>
-      <c r="D11" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:6" ht="14.4">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:11" ht="14.4">
       <c r="A12" s="7">
         <v>9</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="9">
-        <v>5</v>
-      </c>
-      <c r="D12" s="17">
+        <v>8</v>
+      </c>
+      <c r="D12" s="12">
         <v>43106</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" spans="1:6" ht="14.4">
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:11" ht="14.4">
       <c r="A13" s="10">
         <v>10</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="16">
+      <c r="C13" s="10">
+        <v>8</v>
+      </c>
+      <c r="D13" s="11">
         <v>43137</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:6" ht="14.4">
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" ht="14.4">
       <c r="A14" s="9"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:6" ht="14.4">
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:11" ht="14.4">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:6" ht="14.4">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:11" ht="14.4">
       <c r="A16" s="10"/>
       <c r="B16" s="8"/>
       <c r="C16" s="10"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="14.4">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="14.4">
       <c r="A18" s="10"/>
       <c r="B18" s="8"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="14.4">
       <c r="A19" s="9"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" ht="14.4">
       <c r="A20" s="10"/>
       <c r="B20" s="8"/>
       <c r="C20" s="10"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="D4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>